<commit_message>
added comma separation to large numbers
</commit_message>
<xml_diff>
--- a/private/ycdb-hydraulic-properties/violin-table.xlsx
+++ b/private/ycdb-hydraulic-properties/violin-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sync\@owrc\pages\snapshots\private\ycdb-hydraulic-properties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5009730-9A23-4119-95D6-88127FC27C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C5B1E1-4E65-4CFE-A797-60E03C441CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24687197-E253-4CA7-99EE-E7B697DCBBFA}"/>
   </bookViews>
@@ -515,8 +515,8 @@
         <v>2.1469999999999999E-6</v>
       </c>
       <c r="H1" t="str">
-        <f>CONCATENATE("| ",B1," | ",C1," | ",D1," | ",TEXT(E1,"0.00E+00")," | ",TEXT(F1,"0.0E+00")," | ",TEXT(G1,"0.0E+00")," |")</f>
-        <v>| Late Stage Glaciolacustrine-Glaciofluvial | K | 14 | 2.45E-05 | 1.2E-06 | 2.1E-06 |</v>
+        <f>CONCATENATE("| ",B1," | ",C1," | ",TEXT(D1,"#,##0")," | ",TEXT(E1,"0.0E+00")," | ",TEXT(F1,"0.0E+00")," | ",TEXT(G1,"0.0E+00")," |")</f>
+        <v>| Late Stage Glaciolacustrine-Glaciofluvial | K | 14 | 2.5E-05 | 1.2E-06 | 2.1E-06 |</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -540,8 +540,8 @@
         <v>1.5153709999999999E-4</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE("| ",B2," | ",C2," | ",D2," | ",TEXT(E2,"0.00E+00")," | ",TEXT(F2,"0.0E+00")," | ",TEXT(G2,"0.0E+00")," |")</f>
-        <v>|  | KSC_SCR | 3417 | 1.11E-03 | 1.2E-04 | 1.5E-04 |</v>
+        <f t="shared" ref="H2:H24" si="0">CONCATENATE("| ",B2," | ",C2," | ",TEXT(D2,"#,##0")," | ",TEXT(E2,"0.0E+00")," | ",TEXT(F2,"0.0E+00")," | ",TEXT(G2,"0.0E+00")," |")</f>
+        <v>|  | KSC_SCR | 3,417 | 1.1E-03 | 1.2E-04 | 1.5E-04 |</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -567,8 +567,8 @@
         <v>2E-8</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H24" si="0">CONCATENATE("| ",B3," | ",C3," | ",D3," | ",TEXT(E3,"0.00E+00")," | ",TEXT(F3,"0.0E+00")," | ",TEXT(G3,"0.0E+00")," |")</f>
-        <v>| Halton Till | K | 106 | 1.54E-05 | 2.4E-08 | 2.0E-08 |</v>
+        <f t="shared" si="0"/>
+        <v>| Halton Till | K | 106 | 1.5E-05 | 2.4E-08 | 2.0E-08 |</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -593,7 +593,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 1446 | 1.24E-03 | 3.2E-04 | 3.7E-04 |</v>
+        <v>|  | KSC_SCR | 1,446 | 1.2E-03 | 3.2E-04 | 3.7E-04 |</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>| Mackinaw/Oak Ridges | K | 152 | 1.70E-04 | 5.4E-06 | 6.7E-06 |</v>
+        <v>| Mackinaw/Oak Ridges | K | 152 | 1.7E-04 | 5.4E-06 | 6.7E-06 |</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -645,7 +645,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 13942 | 6.59E-04 | 1.6E-04 | 1.5E-04 |</v>
+        <v>|  | KSC_SCR | 13,942 | 6.6E-04 | 1.6E-04 | 1.5E-04 |</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -672,7 +672,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>| Channel - Silt | K | 18 | 9.48E-06 | 5.7E-07 | 1.1E-06 |</v>
+        <v>| Channel - Silt | K | 18 | 9.5E-06 | 5.7E-07 | 1.1E-06 |</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 873 | 5.68E-04 | 1.3E-04 | 1.2E-04 |</v>
+        <v>|  | KSC_SCR | 873 | 5.7E-04 | 1.3E-04 | 1.2E-04 |</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -724,7 +724,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>| Channel - Sand | K | 10 | 4.67E-05 | 5.5E-06 | 1.9E-05 |</v>
+        <v>| Channel - Sand | K | 10 | 4.7E-05 | 5.5E-06 | 1.9E-05 |</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -749,7 +749,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 1389 | 6.00E-04 | 1.2E-04 | 9.9E-05 |</v>
+        <v>|  | KSC_SCR | 1,389 | 6.0E-04 | 1.2E-04 | 9.9E-05 |</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -776,7 +776,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>| Upper Newmarket | K | 19 | 1.02E-05 | 3.3E-07 | 3.4E-07 |</v>
+        <v>| Upper Newmarket | K | 19 | 1.0E-05 | 3.3E-07 | 3.4E-07 |</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -801,7 +801,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 13734 | 7.50E-04 | 2.0E-04 | 1.9E-04 |</v>
+        <v>|  | KSC_SCR | 13,734 | 7.5E-04 | 2.0E-04 | 1.9E-04 |</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -828,7 +828,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>| Inter Newmarket Sediment | K | 21 | 4.01E-04 | 3.5E-06 | 1.0E-06 |</v>
+        <v>| Inter Newmarket Sediment | K | 21 | 4.0E-04 | 3.5E-06 | 1.0E-06 |</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 6111 | 9.74E-04 | 2.1E-04 | 2.1E-04 |</v>
+        <v>|  | KSC_SCR | 6,111 | 9.7E-04 | 2.1E-04 | 2.1E-04 |</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -880,7 +880,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>| Lower Newmarket | K | 61 | 1.83E-04 | 4.4E-07 | 7.7E-07 |</v>
+        <v>| Lower Newmarket | K | 61 | 1.8E-04 | 4.4E-07 | 7.7E-07 |</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -905,7 +905,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 11657 | 8.81E-04 | 2.1E-04 | 2.2E-04 |</v>
+        <v>|  | KSC_SCR | 11,657 | 8.8E-04 | 2.1E-04 | 2.2E-04 |</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -932,7 +932,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>| Thorncliffe | K | 79 | 6.04E-04 | 1.8E-05 | 3.3E-05 |</v>
+        <v>| Thorncliffe | K | 79 | 6.0E-04 | 1.8E-05 | 3.3E-05 |</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -957,7 +957,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 10254 | 6.43E-04 | 1.1E-04 | 1.0E-04 |</v>
+        <v>|  | KSC_SCR | 10,254 | 6.4E-04 | 1.1E-04 | 1.0E-04 |</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -984,7 +984,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>| Sunnybrook | K | 1 | 9.11E-07 | 9.1E-07 | 9.1E-07 |</v>
+        <v>| Sunnybrook | K | 1 | 9.1E-07 | 9.1E-07 | 9.1E-07 |</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1009,7 +1009,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 6971 | 4.62E-04 | 1.1E-04 | 1.1E-04 |</v>
+        <v>|  | KSC_SCR | 6,971 | 4.6E-04 | 1.1E-04 | 1.1E-04 |</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>| Scarborough | K | 31 | 3.51E-04 | 2.4E-05 | 9.2E-05 |</v>
+        <v>| Scarborough | K | 31 | 3.5E-04 | 2.4E-05 | 9.2E-05 |</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 6928 | 6.90E-04 | 1.1E-04 | 1.2E-04 |</v>
+        <v>|  | KSC_SCR | 6,928 | 6.9E-04 | 1.1E-04 | 1.2E-04 |</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>| Bedrock - Undifferentiated | K | 53 | 2.23E-05 | 7.1E-07 | 1.0E-06 |</v>
+        <v>| Bedrock - Undifferentiated | K | 53 | 2.2E-05 | 7.1E-07 | 1.0E-06 |</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>|  | KSC_SCR | 77114 | 5.33E-04 | 1.7E-05 | 1.7E-05 |</v>
+        <v>|  | KSC_SCR | 77,114 | 5.3E-04 | 1.7E-05 | 1.7E-05 |</v>
       </c>
     </row>
   </sheetData>

</xml_diff>